<commit_message>
BFI IAT - Processing Part done
nearly done with the processing part
undone:
- filling the codebook
- better comments and html
</commit_message>
<xml_diff>
--- a/personality and race-IAT study/data/processed/data_processed_codebook.xlsx
+++ b/personality and race-IAT study/data/processed/data_processed_codebook.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -89,6 +89,9 @@
     <t xml:space="preserve">bfi_o1</t>
   </si>
   <si>
+    <t xml:space="preserve">bfi_o10</t>
+  </si>
+  <si>
     <t xml:space="preserve">bfi_o2</t>
   </si>
   <si>
@@ -113,6 +116,33 @@
     <t xml:space="preserve">bfi_o9</t>
   </si>
   <si>
+    <t xml:space="preserve">bfi_c1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_c2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_c3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_c4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_c5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_c6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_c7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_c8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_c9</t>
+  </si>
+  <si>
     <t xml:space="preserve">bfi_e1</t>
   </si>
   <si>
@@ -159,33 +189,6 @@
   </si>
   <si>
     <t xml:space="preserve">bfi_n8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_c1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_c2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_c3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_c4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_c5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_c6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_c7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_c8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bfi_c9</t>
   </si>
   <si>
     <t xml:space="preserve">exclude_impossible</t>
@@ -933,6 +936,12 @@
       </c>
       <c r="B65"/>
     </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
finished the Task for BFI and IAT
commentary done
formating
knitting
</commit_message>
<xml_diff>
--- a/personality and race-IAT study/data/processed/data_processed_codebook.xlsx
+++ b/personality and race-IAT study/data/processed/data_processed_codebook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tina\Documents\GitHub\dpm-assignments\personality and race-IAT study\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB18762-59D5-4E36-A0E6-43FFAA0DD7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840F6867-305F-4816-B53D-E7C1E973EE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="94">
   <si>
     <t>variable</t>
   </si>
@@ -223,90 +223,101 @@
     <t>exclude_participant</t>
   </si>
   <si>
-    <t>Jede Versuchsperson hat ihre persönliche ID, um ihre Daten zueinander zuzordnen</t>
-  </si>
-  <si>
-    <t>Der Durchschnitt der Reaktionszeit einer Versuchsperson aus den Trial blocks 3 und 6.</t>
-  </si>
-  <si>
-    <t>Der Durchschnitt der Reaktionszeit einer Versuchsperson aus den Trial blocks 4 und 7.</t>
-  </si>
-  <si>
-    <t>Greenwald D, Effektgrösse, (D = (mean2 - mean1)/SD), einer Versuchsperson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD von den Raktionszeiten in blocks 3, 4, 6 and 7, wurde für die Berechnung des Greenwald D benötigt, von einer Versuchsperson </t>
-  </si>
-  <si>
-    <t>diese Variable wurde gebildet, um herauszufinden ob die Versuchsperson alle Trials durchlaufen ist (insgesamt 120)</t>
-  </si>
-  <si>
-    <t>Falls die Versuchsperson in "total_trials" nicht 120 hatte, dann wurde sie excluded</t>
-  </si>
-  <si>
-    <t>Berechnet den Durchschnitt, wie oft eine Versuchsperson in ihr Trials die korrekte Antwort gegeben hat</t>
-  </si>
-  <si>
-    <t>diese Variable berechnet den Durchschnitt wie viele der Trials unter 300 ms sind</t>
-  </si>
-  <si>
-    <t>diese Variable excludiert Versuchspersonen die weniger als 75 % akkurat in ihren Trials waren</t>
-  </si>
-  <si>
-    <t>diese Variable excludiert Versuchspersonen, die eine unmögliche Antwort auf gegeben haben (bsp. 1-6 sind möglich, aber 7 oder 0 unmöglich)</t>
-  </si>
-  <si>
-    <t>Diese Variable excludiert Versuchspersonen, die eunvollständig eine Skala ausgefüllt haben (Achtung: sie excludiert sie nicht, falls sie eine ganze Skala nciht ausgefüllt haben, sondern nur, wenn eine Skala teilweise, aber nciht komplett ausgefüllt ist!)</t>
-  </si>
-  <si>
-    <t>Das ist die Master Exclude Variable, die erfasst ob auf einer der anderen esclud variablen (exclude_impossible, exclude_not_completed, exclude_incomplete, exclude_fast , exclude_accuracy) "exclude" steht und wird es wiedergeben, zusätzlich schliesst sie Versuchspersonen aus, die ihre Demographische Angaben angegeben haben, aber keine der Skalen ausgefüllt haben.</t>
-  </si>
-  <si>
-    <t>[1-6] Item aus der Agreeableness Skala</t>
-  </si>
-  <si>
-    <t>[1-6] Item aus der Openness Skala</t>
-  </si>
-  <si>
     <t>[1-6] Item aus der Conscientiousness Skala</t>
   </si>
   <si>
-    <t>[1-6] Item aus der Extraversion Skala</t>
-  </si>
-  <si>
-    <t>[1-6] Item aus der Neurotizimus Skala</t>
-  </si>
-  <si>
-    <t>das Alter der Versuchsperso (war nicht obligatorisch)</t>
-  </si>
-  <si>
-    <t>das Geschlecht der Versuchsperson (war nicht obligatorisch)</t>
-  </si>
-  <si>
-    <t>Der Durchschnittswert einer Versuchsperson, die die Agreeablness Skala ausgefüllt hat. (alle bfi_a items/ durch die Anzahl der Items)</t>
-  </si>
-  <si>
-    <t>Der Durchschnittswert einer Versuchsperson, die die Openness Skala ausgefüllt hat.  (alle bfi_o items/ durch die Anzahl der Items)</t>
-  </si>
-  <si>
-    <t>Der Durchschnittswert einer Versuchsperson, die die Extraversion Skala ausgefüllt hat.  (alle bfi_e items/ durch die Anzahl der Items)</t>
-  </si>
-  <si>
-    <t>Der Durchschnittswert einer Versuchsperson, die die Neuroticismus Skala ausgefüllt hat.  (alle bfi_n items/ durch die Anzahl der Items)</t>
-  </si>
-  <si>
-    <t>Der Durchschnittswert einer Versuchsperson, die die Consci... Skala ausgefüllt hat.  (alle bfi_c items/ durch die Anzahl der Items)</t>
-  </si>
-  <si>
-    <t>diese Variable excluded die Versuchspersonen, die mehr als 10% of the  trials are &lt; 300ms</t>
+    <t>Each test subject has their own personal ID to match their data to each other</t>
+  </si>
+  <si>
+    <t>The average reaction time of a test subject from trial blocks 3 and 6.</t>
+  </si>
+  <si>
+    <t>The average reaction time of a test subject from trial blocks 4 and 7.</t>
+  </si>
+  <si>
+    <t>The gender of the test subject (was not mandatory).</t>
+  </si>
+  <si>
+    <t>The age of the test person (was not mandatory).</t>
+  </si>
+  <si>
+    <t>SD of the reaction times in blocks 3, 4, 6 and 7, was required for the calculation of the Greenwald D, from one subject.</t>
+  </si>
+  <si>
+    <t>Greenwald D, effect size, (D = (mean2 - mean1)/SD), of one subject.</t>
+  </si>
+  <si>
+    <t>This variable was created to find out whether the subject had completed all trials (120 in total).</t>
+  </si>
+  <si>
+    <t>If the test subject did not have 120 in "total_trials", then it was excluded.</t>
+  </si>
+  <si>
+    <t>This variable notes the average of how many of the trials are under 300 ms.</t>
+  </si>
+  <si>
+    <t>Notes the average number of times a subject has given the correct answer in their trial.</t>
+  </si>
+  <si>
+    <t>This variable excludes the subjects who had more than 10% of the trials &lt; 300ms.</t>
+  </si>
+  <si>
+    <t>This variable excludes subjects who had less than 75% accurate in their trials.</t>
+  </si>
+  <si>
+    <t>[1-6] Item from the Agreeableness Scale</t>
+  </si>
+  <si>
+    <t>[1-6] Item from the Openness Scale</t>
+  </si>
+  <si>
+    <t>[1-6] Item from the Conscientiousness Scale</t>
+  </si>
+  <si>
+    <t>[1-6] Item from the Extraversion Scale</t>
+  </si>
+  <si>
+    <t>[1-6] Item from the Neuroticism Scale</t>
+  </si>
+  <si>
+    <t>This is the master exclude variable, which notes whether one of the other exclude variables (exclude_impossible, exclude_not_completed, exclude_incomplete, exclude_fast, exclude_accuracy) says "exclude", in addition it excludes subjects who have given their demographic information but have not completed any of the scales.</t>
+  </si>
+  <si>
+    <t>The average score of a subject who completed the Neuroticism Scale.  (all bfi_n items/ by the number of items)</t>
+  </si>
+  <si>
+    <t>The average score of a subject who completed the Extraversion Scale.  (all bfi_e items/ by the number of items).</t>
+  </si>
+  <si>
+    <t>The average score of a subject who completed the Openness Scale.  (all bfi_o items/ divided by the number of items).</t>
+  </si>
+  <si>
+    <t>The average score of a subject who completed the Agreeableness Scale. (all bfi_a items/ by the number of items).</t>
+  </si>
+  <si>
+    <t>This variable excludes subjects who have incompletely filled out a scale (note: it does not exclude them if they have not filled out an entire scale, but only if a scale is partially but not completely filled out!).</t>
+  </si>
+  <si>
+    <t>This variable excludes subjects who have given an impossible answer (e.g. 1-6 are possible, but 7 or 0 are impossible).</t>
+  </si>
+  <si>
+    <t>The average score of a subject who completed the Conscientiousness Scale.  (all bfi_c items/ divided by the number of items).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -334,8 +345,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -635,7 +648,7 @@
   <dimension ref="A1:B66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="R55" sqref="R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,10 +657,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -656,7 +669,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -664,7 +677,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -672,7 +685,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -680,7 +693,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -688,7 +701,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -696,7 +709,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -704,7 +717,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -712,7 +725,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -720,7 +733,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -728,7 +741,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -736,7 +749,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -744,7 +757,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -752,15 +765,15 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
-        <v>80</v>
+      <c r="B15" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -768,7 +781,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -776,7 +789,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -784,7 +797,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -792,7 +805,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -800,7 +813,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -808,7 +821,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -816,7 +829,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -824,15 +837,15 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B24" t="s">
-        <v>81</v>
+      <c r="B24" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -840,7 +853,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -848,7 +861,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -856,7 +869,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -864,7 +877,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -872,7 +885,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -880,7 +893,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -888,7 +901,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -896,7 +909,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -904,23 +917,23 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
-      <c r="B34" t="s">
-        <v>82</v>
+      <c r="B34" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="B35" t="s">
-        <v>82</v>
+      <c r="B35" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -928,7 +941,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -936,7 +949,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -944,7 +957,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -952,7 +965,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -960,7 +973,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -968,7 +981,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -976,15 +989,15 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
-      <c r="B43" t="s">
-        <v>83</v>
+      <c r="B43" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -992,7 +1005,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1000,7 +1013,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1008,7 +1021,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1016,7 +1029,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1024,7 +1037,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1032,7 +1045,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1040,15 +1053,15 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
-      <c r="B51" t="s">
-        <v>84</v>
+      <c r="B51" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1056,7 +1069,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1064,7 +1077,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1072,7 +1085,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1080,7 +1093,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1088,7 +1101,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1096,7 +1109,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1104,7 +1117,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1112,7 +1125,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1120,7 +1133,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1128,7 +1141,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1136,7 +1149,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1144,7 +1157,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1152,7 +1165,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1160,7 +1173,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1168,11 +1181,11 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>